<commit_message>
Refactored some rust, displaying fields nicer in svelte + clipboard + notifications.
</commit_message>
<xml_diff>
--- a/testing/data.xlsx
+++ b/testing/data.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samwillis/Projects/searcher-rs/testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B921A985-0C3B-724D-B9A1-069F800DE77E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11637E0-1339-D143-B803-1C49449D4EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4120" yWindow="760" windowWidth="28040" windowHeight="16380" xr2:uid="{B974D151-D769-F648-9BC6-E8FAE924C891}"/>
+    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16380" activeTab="1" xr2:uid="{B974D151-D769-F648-9BC6-E8FAE924C891}"/>
   </bookViews>
   <sheets>
     <sheet name="My Data" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="22">
   <si>
     <t>Code</t>
   </si>
@@ -67,16 +68,58 @@
   </si>
   <si>
     <t>Testing Testing Testing</t>
+  </si>
+  <si>
+    <t>124 Name</t>
+  </si>
+  <si>
+    <t>125 Name</t>
+  </si>
+  <si>
+    <t>126 Name</t>
+  </si>
+  <si>
+    <t>127 Name</t>
+  </si>
+  <si>
+    <t>128 Name</t>
+  </si>
+  <si>
+    <t>129 Name</t>
+  </si>
+  <si>
+    <t>130 Name</t>
+  </si>
+  <si>
+    <t>131 Name</t>
+  </si>
+  <si>
+    <t>132 Name</t>
+  </si>
+  <si>
+    <t>as</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>d</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -418,40 +461,100 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D22CEE61-2306-044A-9017-CBC4111848FE}">
-  <dimension ref="A4:F5"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>123</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>1230897</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>124</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>1230897</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>0</v>
+      <c r="A4">
+        <v>125</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
+        <v>11</v>
+      </c>
+      <c r="C4">
+        <v>1230897</v>
       </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C5">
         <v>1230897</v>
@@ -466,19 +569,251 @@
         <v>9</v>
       </c>
     </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>127</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>1230897</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>128</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>1230897</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>129</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>1230897</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>130</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9">
+        <v>1230897</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>131</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10">
+        <v>1230897</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>132</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11">
+        <v>1230897</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ACFFA94-09ED-FA4C-BB67-F437A8E45742}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>123</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <v>1230897</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>124</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>1230897</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>125</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>1230897</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>